<commit_message>
v3.6 excel i admin
* Zatwierdzanie badania w tabeli wszytskie badania podczas dodawania z excela

* Logowanie sprawdza też tabelę kont administratorów

* logowanie na konto administratora
</commit_message>
<xml_diff>
--- a/excel/analizator_kwasu_mlekowego.xlsx
+++ b/excel/analizator_kwasu_mlekowego.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>data</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>6.69</t>
   </si>
 </sst>
 </file>
@@ -351,7 +348,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -362,7 +359,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -393,13 +390,9 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1">
-        <v>7</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>

</xml_diff>